<commit_message>
refactor: Update MIGO test case and improve Excel data handling
</commit_message>
<xml_diff>
--- a/Dados/Dados apresentação 22-08.xlsx
+++ b/Dados/Dados apresentação 22-08.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vibraenergia-my.sharepoint.com/personal/caiofernandes_vibraenergia_com_br/Documents/Documentos/testeS4-main/Caso run/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vibraenergia-my.sharepoint.com/personal/josemichael_vibraenergia_com_br/Documents/Documentos/GitHub/testeS4/Dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF29D3F6-DF1E-42AF-973A-BCAFDB44CB0C}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E33BC99C-6945-4FEA-891D-BD9D54600526}"/>
   <bookViews>
-    <workbookView xWindow="-3015" yWindow="-11490" windowWidth="24300" windowHeight="7740" xr2:uid="{01F98A4B-07BB-472F-82FB-B59EC1EF1266}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{01F98A4B-07BB-472F-82FB-B59EC1EF1266}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
-  <si>
-    <t>Pedido Origen</t>
-  </si>
-  <si>
-    <t>Novo Pedido</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>TIP DE PEDIDO</t>
   </si>
@@ -80,9 +74,6 @@
     <t>Data de Remessa</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>ZD</t>
   </si>
   <si>
@@ -98,9 +89,6 @@
     <t>BACUB Base de Cubatão</t>
   </si>
   <si>
-    <t>OK</t>
-  </si>
-  <si>
     <t>01.008.166</t>
   </si>
   <si>
@@ -116,20 +104,32 @@
     <t>Preço</t>
   </si>
   <si>
-    <t>TIP DE CONTRATO</t>
-  </si>
-  <si>
     <t>ZDDR</t>
   </si>
   <si>
-    <t>NOVO CONTRATO</t>
+    <t>TP CONTRATO</t>
+  </si>
+  <si>
+    <t>NV CONTRATO</t>
+  </si>
+  <si>
+    <t>NV PEDIDO</t>
+  </si>
+  <si>
+    <t>MIGO</t>
+  </si>
+  <si>
+    <t>MIRO</t>
+  </si>
+  <si>
+    <t>Pedido Origem</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,8 +145,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,12 +170,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -198,9 +200,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,104 +535,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8A3E43-7AED-4335-9954-9B9CBBFD2381}">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="16" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="P1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="S1" s="4" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>4503273185</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="1">
+        <v>6</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1">
         <v>10001859</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1">
         <v>5821</v>
@@ -644,47 +648,45 @@
         <v>2000</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="K2" s="1">
         <v>602.13800000000003</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="N2" s="1">
         <v>50</v>
       </c>
       <c r="O2" s="2">
         <v>45899</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>6</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>4503274856</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1">
+        <v>7</v>
+      </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1">
         <v>10068989</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G3" s="1">
         <v>5821</v>
@@ -696,30 +698,29 @@
         <v>2000</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K3" s="1">
         <v>120</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="1"/>
       <c r="N3" s="1">
         <v>60</v>
       </c>
       <c r="O3" s="2">
         <v>45899</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>7</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="L8" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
refactor: Update MIGO test case to use new Excel column references and improve error handling
</commit_message>
<xml_diff>
--- a/Dados/Dados apresentação 22-08.xlsx
+++ b/Dados/Dados apresentação 22-08.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vibraenergia-my.sharepoint.com/personal/josemichael_vibraenergia_com_br/Documents/Documentos/GitHub/testeS4/Dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E33BC99C-6945-4FEA-891D-BD9D54600526}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3A17001-B7E3-5605-A007-67720D0FFEE6}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{01F98A4B-07BB-472F-82FB-B59EC1EF1266}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>TIP DE PEDIDO</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>Pedido Origem</t>
+  </si>
+  <si>
+    <t>ipo documento</t>
   </si>
 </sst>
 </file>
@@ -537,7 +540,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8A3E43-7AED-4335-9954-9B9CBBFD2381}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -707,7 +712,7 @@
         <v>18</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="N3" s="1">
         <v>60</v>

</xml_diff>

<commit_message>
refactor: Adjust contract number extraction length in VBS script
</commit_message>
<xml_diff>
--- a/Dados/Dados apresentação 22-08.xlsx
+++ b/Dados/Dados apresentação 22-08.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vibraenergia-my.sharepoint.com/personal/josemichael_vibraenergia_com_br/Documents/Documentos/GitHub/testeS4/Dados/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vibraenergia-my.sharepoint.com/personal/caiofernandes_vibraenergia_com_br/Documents/Documentos/testeS4/Dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3A17001-B7E3-5605-A007-67720D0FFEE6}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{858893E2-B412-411C-AF97-8AF5F88A5E5C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{01F98A4B-07BB-472F-82FB-B59EC1EF1266}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="15375" windowHeight="7785" xr2:uid="{01F98A4B-07BB-472F-82FB-B59EC1EF1266}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -540,32 +540,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8A3E43-7AED-4335-9954-9B9CBBFD2381}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="16" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -624,7 +624,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>4503273185</v>
       </c>
@@ -670,11 +670,13 @@
       <c r="O2" s="2">
         <v>45899</v>
       </c>
-      <c r="P2" s="1"/>
+      <c r="P2" s="1">
+        <v>4600244207</v>
+      </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>4503274856</v>
       </c>
@@ -724,7 +726,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L8" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: Enhance Excel handling in CRIAR_PEDIDOS.vbs to ensure proper closure and saving of workbooks
</commit_message>
<xml_diff>
--- a/Dados/Dados apresentação 22-08.xlsx
+++ b/Dados/Dados apresentação 22-08.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vibraenergia-my.sharepoint.com/personal/caiofernandes_vibraenergia_com_br/Documents/Documentos/testeS4/Dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{858893E2-B412-411C-AF97-8AF5F88A5E5C}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1878311-3027-41EF-9933-2238E35560CB}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="1860" windowWidth="15375" windowHeight="7785" xr2:uid="{01F98A4B-07BB-472F-82FB-B59EC1EF1266}"/>
   </bookViews>
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8A3E43-7AED-4335-9954-9B9CBBFD2381}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,9 +671,11 @@
         <v>45899</v>
       </c>
       <c r="P2" s="1">
-        <v>4600244207</v>
-      </c>
-      <c r="Q2" s="1"/>
+        <v>4600244209</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>4503342003</v>
+      </c>
       <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -722,8 +724,12 @@
       <c r="O3" s="2">
         <v>45899</v>
       </c>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
+      <c r="P3" s="1">
+        <v>4600244210</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>4503342004</v>
+      </c>
       <c r="R3" s="1"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add constants for density and temperature; update MIGO test case to handle zero values
- Introduced constants ${DENSIDADE} and ${TEMP} for density and temperature.
- Updated the MIGO test case to include checks for zero values in material temperature and test density.
- Enhanced logging and error handling in the test execution process.
- Fixed issues related to opening the Excel workbook and reading test data.
- Updated output files to reflect changes in test execution and results.
</commit_message>
<xml_diff>
--- a/Dados/Dados apresentação 22-08.xlsx
+++ b/Dados/Dados apresentação 22-08.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vibraenergia-my.sharepoint.com/personal/josemichael_vibraenergia_com_br/Documents/Documentos/GitHub/testeS4/Dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3A17001-B7E3-5605-A007-67720D0FFEE6}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9416700-E5BD-4C05-A2E3-BEA91C1F0759}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{01F98A4B-07BB-472F-82FB-B59EC1EF1266}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>TIP DE PEDIDO</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>Pedido Origem</t>
-  </si>
-  <si>
-    <t>ipo documento</t>
   </si>
 </sst>
 </file>
@@ -540,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8A3E43-7AED-4335-9954-9B9CBBFD2381}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -664,14 +661,16 @@
       <c r="M2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="1">
-        <v>50</v>
-      </c>
+      <c r="N2" s="1"/>
       <c r="O2" s="2">
         <v>45899</v>
       </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
+      <c r="P2" s="1">
+        <v>4600244205</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>4503342001</v>
+      </c>
       <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
@@ -712,16 +711,18 @@
         <v>18</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" s="1">
-        <v>60</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="N3" s="1"/>
       <c r="O3" s="2">
         <v>45899</v>
       </c>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
+      <c r="P3" s="1">
+        <v>4600244206</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>4503342002</v>
+      </c>
       <c r="R3" s="1"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
refactor: Improve contract creation script by adding price handling and optimizing workflow
</commit_message>
<xml_diff>
--- a/Dados/Dados apresentação 22-08.xlsx
+++ b/Dados/Dados apresentação 22-08.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vibraenergia-my.sharepoint.com/personal/caiofernandes_vibraenergia_com_br/Documents/Documentos/testeS4/Dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1878311-3027-41EF-9933-2238E35560CB}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCC68978-362D-4927-92F2-E8093F5A2BD1}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="15375" windowHeight="7785" xr2:uid="{01F98A4B-07BB-472F-82FB-B59EC1EF1266}"/>
+    <workbookView xWindow="23415" yWindow="1020" windowWidth="24915" windowHeight="7785" xr2:uid="{01F98A4B-07BB-472F-82FB-B59EC1EF1266}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>TIP DE PEDIDO</t>
   </si>
@@ -77,9 +77,6 @@
     <t>ZD</t>
   </si>
   <si>
-    <t>ZCTP</t>
-  </si>
-  <si>
     <t>Z13</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>BAPLAN Base de Paulínia</t>
   </si>
   <si>
-    <t>A003</t>
-  </si>
-  <si>
     <t>Z10</t>
   </si>
   <si>
@@ -125,7 +119,7 @@
     <t>Pedido Origem</t>
   </si>
   <si>
-    <t>ipo documento</t>
+    <t>Z000</t>
   </si>
 </sst>
 </file>
@@ -540,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8A3E43-7AED-4335-9954-9B9CBBFD2381}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,10 +561,10 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -603,7 +597,7 @@
         <v>9</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>10</v>
@@ -612,16 +606,16 @@
         <v>11</v>
       </c>
       <c r="P1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -638,10 +632,10 @@
         <v>10001859</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="G2" s="1">
         <v>5821</v>
@@ -653,29 +647,25 @@
         <v>2000</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K2" s="1">
         <v>602.13800000000003</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="1">
-        <v>50</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="N2" s="1"/>
       <c r="O2" s="2">
         <v>45899</v>
       </c>
       <c r="P2" s="1">
-        <v>4600244209</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>4503342003</v>
-      </c>
+        <v>4600244273</v>
+      </c>
+      <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -692,10 +682,10 @@
         <v>10068989</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G3" s="1">
         <v>5821</v>
@@ -707,29 +697,23 @@
         <v>2000</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K3" s="1">
         <v>120</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" s="1">
-        <v>60</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="N3" s="1"/>
       <c r="O3" s="2">
         <v>45899</v>
       </c>
-      <c r="P3" s="1">
-        <v>4600244210</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>4503342004</v>
-      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update MIGO test output and report files with new execution timestamps and error messages.
</commit_message>
<xml_diff>
--- a/Dados/Dados apresentação 22-08.xlsx
+++ b/Dados/Dados apresentação 22-08.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vibraenergia-my.sharepoint.com/personal/josemichael_vibraenergia_com_br/Documents/Documentos/GitHub/testeS4/Dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9416700-E5BD-4C05-A2E3-BEA91C1F0759}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{174B5A2A-7DB7-4EED-8078-8C3ED8E1FB01}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{01F98A4B-07BB-472F-82FB-B59EC1EF1266}"/>
+    <workbookView xWindow="9615" yWindow="3555" windowWidth="14340" windowHeight="7245" xr2:uid="{01F98A4B-07BB-472F-82FB-B59EC1EF1266}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -537,32 +537,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8A3E43-7AED-4335-9954-9B9CBBFD2381}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="16" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
@@ -621,7 +621,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>4503273185</v>
       </c>
@@ -666,14 +666,14 @@
         <v>45899</v>
       </c>
       <c r="P2" s="1">
-        <v>4600244205</v>
+        <v>4600244240</v>
       </c>
       <c r="Q2" s="1">
-        <v>4503342001</v>
+        <v>4503342033</v>
       </c>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>4503274856</v>
       </c>
@@ -718,14 +718,14 @@
         <v>45899</v>
       </c>
       <c r="P3" s="1">
-        <v>4600244206</v>
+        <v>4600244241</v>
       </c>
       <c r="Q3" s="1">
-        <v>4503342002</v>
+        <v>4503342035</v>
       </c>
       <c r="R3" s="1"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L8" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: Simplify contract handling logic in order processing script
</commit_message>
<xml_diff>
--- a/Dados/Dados apresentação 22-08.xlsx
+++ b/Dados/Dados apresentação 22-08.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vibraenergia-my.sharepoint.com/personal/caiofernandes_vibraenergia_com_br/Documents/Documentos/testeS4/Dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48FE72C3-A02D-40E3-A435-57913ACEF46C}"/>
+  <xr:revisionPtr revIDLastSave="162" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68A3C6EC-1783-4620-A367-F6B0312039B1}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="23415" yWindow="1020" windowWidth="24915" windowHeight="7785" xr2:uid="{01F98A4B-07BB-472F-82FB-B59EC1EF1266}"/>
+    <workbookView xWindow="22410" yWindow="1290" windowWidth="24915" windowHeight="7785" xr2:uid="{01F98A4B-07BB-472F-82FB-B59EC1EF1266}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -535,7 +535,7 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,8 +662,12 @@
       <c r="O2" s="2">
         <v>45899</v>
       </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
+      <c r="P2" s="1">
+        <v>4600244283</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>4503342086</v>
+      </c>
       <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -710,8 +714,12 @@
       <c r="O3" s="2">
         <v>45899</v>
       </c>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
+      <c r="P3" s="1">
+        <v>4600244284</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>4503342087</v>
+      </c>
       <c r="R3" s="1"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
- Updated test suite results to indicate all tests passed successfully. - Modified strings to include additional context for the MIRO transaction.
</commit_message>
<xml_diff>
--- a/Dados/Dados apresentação 22-08.xlsx
+++ b/Dados/Dados apresentação 22-08.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vibraenergia-my.sharepoint.com/personal/josemichael_vibraenergia_com_br/Documents/Documentos/GitHub/testeS4/Dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EAC1112-2613-4352-93F5-D551611220EA}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36EE171A-B187-4D7B-A0C4-6AD49BC0557A}"/>
   <bookViews>
-    <workbookView xWindow="4305" yWindow="2580" windowWidth="23250" windowHeight="7245" xr2:uid="{01F98A4B-07BB-472F-82FB-B59EC1EF1266}"/>
+    <workbookView xWindow="9630" yWindow="3405" windowWidth="15975" windowHeight="7245" xr2:uid="{01F98A4B-07BB-472F-82FB-B59EC1EF1266}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -543,29 +543,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8A3E43-7AED-4335-9954-9B9CBBFD2381}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:Q3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
@@ -672,10 +674,10 @@
         <v>45899</v>
       </c>
       <c r="P2" s="1">
-        <v>4600244281</v>
+        <v>4600244316</v>
       </c>
       <c r="Q2" s="1">
-        <v>4503342051</v>
+        <v>4503342084</v>
       </c>
       <c r="R2" s="1"/>
     </row>
@@ -724,10 +726,10 @@
         <v>45899</v>
       </c>
       <c r="P3" s="1">
-        <v>4600244282</v>
+        <v>4600244317</v>
       </c>
       <c r="Q3" s="1">
-        <v>4503342052</v>
+        <v>4503342085</v>
       </c>
       <c r="R3" s="1"/>
     </row>

</xml_diff>

<commit_message>
refactor: Update order creation logic in CRIAR_PEDIDOS.vbs for improved data handling
</commit_message>
<xml_diff>
--- a/Dados/Dados apresentação 22-08.xlsx
+++ b/Dados/Dados apresentação 22-08.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vibraenergia-my.sharepoint.com/personal/caiofernandes_vibraenergia_com_br/Documents/Documentos/testeS4/Dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="162" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68A3C6EC-1783-4620-A367-F6B0312039B1}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26A4AC83-EEDB-4711-9741-C93EB33B3E86}"/>
   <bookViews>
-    <workbookView xWindow="22410" yWindow="1290" windowWidth="24915" windowHeight="7785" xr2:uid="{01F98A4B-07BB-472F-82FB-B59EC1EF1266}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="345" windowWidth="20655" windowHeight="5970" xr2:uid="{01F98A4B-07BB-472F-82FB-B59EC1EF1266}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -213,6 +213,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -534,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8A3E43-7AED-4335-9954-9B9CBBFD2381}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,8 +669,8 @@
       <c r="P2" s="1">
         <v>4600244283</v>
       </c>
-      <c r="Q2" s="1">
-        <v>4503342086</v>
+      <c r="Q2">
+        <v>4503342107</v>
       </c>
       <c r="R2" s="1"/>
     </row>
@@ -718,7 +722,7 @@
         <v>4600244284</v>
       </c>
       <c r="Q3" s="1">
-        <v>4503342087</v>
+        <v>4503342108</v>
       </c>
       <c r="R3" s="1"/>
     </row>

</xml_diff>

<commit_message>
refactor: Improve error handling and logging in MIGO transaction processing
</commit_message>
<xml_diff>
--- a/Dados/Dados apresentação 22-08.xlsx
+++ b/Dados/Dados apresentação 22-08.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vibraenergia-my.sharepoint.com/personal/josemichael_vibraenergia_com_br/Documents/Documentos/GitHub/testeS4/Dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36EE171A-B187-4D7B-A0C4-6AD49BC0557A}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3432422-EDAA-4394-AF26-6F26210B95A8}"/>
   <bookViews>
-    <workbookView xWindow="9630" yWindow="3405" windowWidth="15975" windowHeight="7245" xr2:uid="{01F98A4B-07BB-472F-82FB-B59EC1EF1266}"/>
+    <workbookView minimized="1" xWindow="2100" yWindow="3270" windowWidth="15975" windowHeight="7245" xr2:uid="{01F98A4B-07BB-472F-82FB-B59EC1EF1266}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -189,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -205,6 +205,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -543,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8A3E43-7AED-4335-9954-9B9CBBFD2381}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,12 +677,12 @@
         <v>45899</v>
       </c>
       <c r="P2" s="1">
-        <v>4600244316</v>
+        <v>4600244328</v>
       </c>
       <c r="Q2" s="1">
-        <v>4503342084</v>
-      </c>
-      <c r="R2" s="1"/>
+        <v>4503342111</v>
+      </c>
+      <c r="R2" s="7"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -726,10 +729,10 @@
         <v>45899</v>
       </c>
       <c r="P3" s="1">
-        <v>4600244317</v>
+        <v>4600244329</v>
       </c>
       <c r="Q3" s="1">
-        <v>4503342085</v>
+        <v>4503342112</v>
       </c>
       <c r="R3" s="1"/>
     </row>

</xml_diff>

<commit_message>
Improves Excel export and error handling for MIRO/MIGO flows
Refactors test automation to accurately export transaction document numbers to specific Excel columns, aligning row indexes with data. Adds missing MIRO result export, groups related operations, and enhances error logging for better traceability during SAP automation.
</commit_message>
<xml_diff>
--- a/Dados/Dados apresentação 22-08.xlsx
+++ b/Dados/Dados apresentação 22-08.xlsx
@@ -2,41 +2,31 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vibraenergia-my.sharepoint.com/personal/josemichael_vibraenergia_com_br/Documents/Documentos/GitHub/testeS4/Dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="8_{8D930324-2335-4E6D-A8B1-E3276BA0CE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3432422-EDAA-4394-AF26-6F26210B95A8}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_DD86054FCB6C7C71BB0FC43E4D6E2FB64806CF2D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58AED8C0-7EB6-4926-AC2D-44940DFA9203}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2100" yWindow="3270" windowWidth="15975" windowHeight="7245" xr2:uid="{01F98A4B-07BB-472F-82FB-B59EC1EF1266}"/>
+    <workbookView xWindow="2100" yWindow="3270" windowWidth="15975" windowHeight="7245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+  <si>
+    <t>Pedido Origem</t>
+  </si>
+  <si>
+    <t>Preço</t>
+  </si>
   <si>
     <t>TIP DE PEDIDO</t>
   </si>
@@ -68,15 +58,33 @@
     <t>CENTRO</t>
   </si>
   <si>
+    <t>TP CONTRATO</t>
+  </si>
+  <si>
     <t>ITEM CONT.</t>
   </si>
   <si>
     <t>Data de Remessa</t>
   </si>
   <si>
+    <t>NV CONTRATO</t>
+  </si>
+  <si>
+    <t>NV PEDIDO</t>
+  </si>
+  <si>
+    <t>MIGO</t>
+  </si>
+  <si>
+    <t>MIRO</t>
+  </si>
+  <si>
     <t>ZD</t>
   </si>
   <si>
+    <t>Z000</t>
+  </si>
+  <si>
     <t>Z13</t>
   </si>
   <si>
@@ -86,47 +94,32 @@
     <t>BACUB Base de Cubatão</t>
   </si>
   <si>
+    <t>ZDDR</t>
+  </si>
+  <si>
+    <t>5014660856</t>
+  </si>
+  <si>
+    <t>5600000372</t>
+  </si>
+  <si>
+    <t>Z10</t>
+  </si>
+  <si>
     <t>01.008.166</t>
   </si>
   <si>
     <t>BAPLAN Base de Paulínia</t>
   </si>
   <si>
-    <t>Z10</t>
-  </si>
-  <si>
-    <t>Preço</t>
-  </si>
-  <si>
-    <t>ZDDR</t>
-  </si>
-  <si>
-    <t>TP CONTRATO</t>
-  </si>
-  <si>
-    <t>NV CONTRATO</t>
-  </si>
-  <si>
-    <t>NV PEDIDO</t>
-  </si>
-  <si>
-    <t>MIGO</t>
-  </si>
-  <si>
-    <t>MIRO</t>
-  </si>
-  <si>
-    <t>Pedido Origem</t>
-  </si>
-  <si>
-    <t>Z000</t>
+    <t>5014660857</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,12 +139,6 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -543,11 +530,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B8A3E43-7AED-4335-9954-9B9CBBFD2381}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,67 +556,66 @@
     <col min="15" max="15" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -640,16 +626,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1">
         <v>10001859</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G2" s="1">
         <v>5821</v>
@@ -661,28 +647,33 @@
         <v>2000</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="K2" s="1">
         <v>602.13800000000003</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="6">
         <v>45899</v>
       </c>
       <c r="P2" s="1">
-        <v>4600244328</v>
+        <v>4600244336</v>
       </c>
       <c r="Q2" s="1">
-        <v>4503342111</v>
-      </c>
-      <c r="R2" s="7"/>
+        <v>4503342117</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="S2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -692,16 +683,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1">
         <v>10068989</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="G3" s="1">
         <v>5821</v>
@@ -713,38 +704,39 @@
         <v>2000</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="K3" s="1">
         <v>120</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="2">
         <v>45899</v>
       </c>
       <c r="P3" s="1">
-        <v>4600244329</v>
+        <v>4600244337</v>
       </c>
       <c r="Q3" s="1">
-        <v>4503342112</v>
-      </c>
-      <c r="R3" s="1"/>
+        <v>4503342118</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L8" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Pública</oddFooter>
+    <oddFooter>&amp;C&amp;"Calibri"&amp;10 &amp;K000000_x000D_# Pública</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>